<commit_message>
Added updated test cases and test plan
</commit_message>
<xml_diff>
--- a/Manual_Test_Cases.xlsx
+++ b/Manual_Test_Cases.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
-  <si>
-    <t>Test Plan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
   </si>
   <si>
     <t>Test Cases</t>
@@ -22,49 +25,58 @@
     <t>Expected Results</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>To make sure the Order module of the e-commerce platform functions correctly -
-meets functional and non-functional requirements, and is prepared for future scalability and integration</t>
-  </si>
-  <si>
     <t>Adding Items to an Order</t>
   </si>
   <si>
-    <t>Add a valid item to the Cart including 
-item name, price, and quantity
-e.g
-("Apple", NOK 1000, quantity 2)</t>
-  </si>
-  <si>
-    <t>Item is added successfully, order list is updated.
-e.g-   (Based on UI/UX design presented on UI) 
-List of items      Qty       Price
-Laptop                2           1000
-Total cost                      NOK 2000</t>
-  </si>
-  <si>
-    <t>Add multiple valid items to the Cart including 
-item name, price, and quantity
-e.g
-("Phone", NOK 500, quantity 1)
-("Tablet", NOK 200, quantity 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Both items are added successfully, order list is updated.
-e.g-   (Based on UI/UX design, presented on UI) 
-List of items      Qty       Price
-Phone                1           500
-Tablet                 2           400
-Total cost                      NOK 900
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>Add valid item to order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open order page. 
+2. Add an item with name, price, and quantity.
 </t>
   </si>
   <si>
-    <t>Add an item with an empty name</t>
-  </si>
-  <si>
-    <t>Error message 
+    <t xml:space="preserve">Item is added successfully, order list is updated with total cost.
+</t>
+  </si>
+  <si>
+    <t>Automate, Manual</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>View order summary</t>
+  </si>
+  <si>
+    <t>1. Add multiple items. 
+2. Navigate to order summary.</t>
+  </si>
+  <si>
+    <t>Displays all items and total cost correctly.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add invalid item (empty name)
+</t>
+  </si>
+  <si>
+    <t>1. Attempt to add an item with an empty name.</t>
+  </si>
+  <si>
+    <t>Error message displayed, item not added.
+Error message 
 "Invalid input: item_name must be non-empty, price and quantity must
 be greater than 0."</t>
   </si>
@@ -72,55 +84,125 @@
     <t>Added error message based on provided code snippet</t>
   </si>
   <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add invalid item (non string value)
+</t>
+  </si>
+  <si>
     <t>Add an item with a non-string value</t>
   </si>
   <si>
-    <t>Error message "Invalid input: item_name must be a string."</t>
+    <t>Error message displayed, item not added.
+Error message "Invalid input: item_name must be a string."</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add invalid item (item name with number)
+</t>
   </si>
   <si>
     <t>Add an item with a number instead of a name (e.g., 123 instead of "Laptop")</t>
   </si>
   <si>
-    <t>Add an item with a negative price (-10) or quantity (-2)</t>
-  </si>
-  <si>
-    <t>Add an item with zero price or quantity</t>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>Add invalid item (negative price)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Attempt to add an item with a negative price.
+</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>Add invalid item (0 price or quantity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Attempt to add an item with a 0 price or quantity 
+</t>
   </si>
   <si>
     <t>Calculating Total Cost</t>
   </si>
   <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>Calculate total cost</t>
+  </si>
+  <si>
     <t>Calculate total after adding multiple valid items</t>
   </si>
   <si>
     <t>Total cost matches sum of all item costs.</t>
   </si>
   <si>
-    <t>Calculate total for an empty order</t>
-  </si>
-  <si>
-    <t>Total should be 0.</t>
-  </si>
-  <si>
-    <t>Verify total when updating item quantities</t>
-  </si>
-  <si>
-    <t>Total updates correctly.</t>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>Empty order total</t>
+  </si>
+  <si>
+    <t>1. Do not add any items. 
+2. Check total cost.</t>
+  </si>
+  <si>
+    <t>Total cost displayed as 0.</t>
   </si>
   <si>
     <t>Non functional Test cases- Performance &amp; Scalability</t>
   </si>
   <si>
+    <t>TC10</t>
+  </si>
+  <si>
     <t>Add 1,000 items to an order and check performance</t>
   </si>
   <si>
     <t>No significant delay in processing.</t>
   </si>
   <si>
+    <t>Automate</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
     <t>Simulate multi-user access (concurrent orders)</t>
   </si>
   <si>
     <t>System handles multiple simultaneous orders without failure.</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>Multi-currency support</t>
+  </si>
+  <si>
+    <t>1. Change currency setting. 
+2. Add item to order.</t>
+  </si>
+  <si>
+    <t>Prices update correctly based on selected currency.</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>Scalability for API integration</t>
+  </si>
+  <si>
+    <t>1. Simulate API calls for inventory, user profiles.</t>
+  </si>
+  <si>
+    <t>APIs interact correctly without breaking order functionality.</t>
   </si>
 </sst>
 </file>
@@ -398,9 +480,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="69.5"/>
-    <col customWidth="1" min="2" max="2" width="41.0"/>
-    <col customWidth="1" min="3" max="3" width="58.5"/>
+    <col customWidth="1" min="1" max="1" width="39.75"/>
+    <col customWidth="1" min="2" max="2" width="30.63"/>
+    <col customWidth="1" min="3" max="3" width="41.0"/>
+    <col customWidth="1" min="4" max="4" width="58.5"/>
+    <col customWidth="1" min="5" max="5" width="33.88"/>
+    <col customWidth="1" min="6" max="6" width="43.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -413,136 +498,262 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
+    </row>
+    <row r="2" ht="35.25" customHeight="1">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11">
-      <c r="B11" s="4" t="s">
-        <v>18</v>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="16">
-      <c r="B16" s="4" t="s">
-        <v>25</v>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="3" t="s">
-        <v>26</v>
+      <c r="A17" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="3" t="s">
-        <v>28</v>
+      <c r="A18" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>